<commit_message>
Update note restanta 2
</commit_message>
<xml_diff>
--- a/Teaching/Biostatistics/results/Tabel_Biostatistica_R2.xlsx
+++ b/Teaching/Biostatistics/results/Tabel_Biostatistica_R2.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -398,9 +398,12 @@
       <c r="D2">
         <v>2</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
       <c r="F2">
         <f>ROUND(SUM(D2,E2),0)+1</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>